<commit_message>
Importador de XLSX implementado
</commit_message>
<xml_diff>
--- a/PlanillaDespachos.xlsx
+++ b/PlanillaDespachos.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Home\Documents\beetrackManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A84E4A-2BA0-4336-9F44-3EBD9D31B29A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869D34DB-6030-437C-B236-F16C8DA3F3F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3D032C6-7964-4F1D-846B-5E1174383D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Despachos" sheetId="1" r:id="rId1"/>
-    <sheet name="NoModificar" sheetId="2" r:id="rId2"/>
+    <sheet name="NoModificar" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Código</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>Retira Luís Hamilton</t>
+  </si>
+  <si>
+    <t>BBV10031256</t>
+  </si>
+  <si>
+    <t>Esteban Gutiérrez</t>
+  </si>
+  <si>
+    <t>Departamental 1455</t>
+  </si>
+  <si>
+    <t>La Florida</t>
   </si>
 </sst>
 </file>
@@ -174,7 +186,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -272,7 +284,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -593,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F628A72-1F90-4074-B106-672B8A70FEC9}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +719,7 @@
       </c>
       <c r="M2" s="7">
         <f ca="1">TODAY()+1</f>
-        <v>44340</v>
+        <v>44342</v>
       </c>
       <c r="N2" t="s">
         <v>22</v>
@@ -752,7 +764,7 @@
       </c>
       <c r="M3" s="7">
         <f ca="1">TODAY()+2</f>
-        <v>44341</v>
+        <v>44343</v>
       </c>
       <c r="N3" t="s">
         <v>21</v>
@@ -764,21 +776,51 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I4" s="6"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5">
+        <v>921635782</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{048A5845-6B8E-46BB-BE31-67A7122AD399}">
+  <dataValidations count="5">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3 E5:E1048576" xr:uid="{56F38AE4-8C89-4CBA-BFB9-5CBCE32390CA}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{4B643240-C193-4E10-847A-DE9AB1C579FA}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3 H5:H1048576" xr:uid="{1E20291B-A013-4973-BD7E-1334BC4AEC0E}">
       <formula1>100000000</formula1>
       <formula2>999999999</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{73C62030-6685-4899-ABD6-A624D493C53D}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3 I5:I1048576" xr:uid="{831CD9A7-4DC9-41F1-BCBD-B4B7EF2B2622}">
       <formula1>ISNUMBER(MATCH("*@*.*",I2,0))</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{EEAF6918-AA93-4284-962F-8D0EE1A9316F}">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{09A9EA9B-9BDB-4566-8E62-594425DCD814}">
+      <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -789,30 +831,36 @@
   <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C27584B5-2E6C-4711-9DF9-2E0EE01F6F1D}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4053D02F-B894-46D0-A410-9E0BCCB2F18A}">
           <x14:formula1>
             <xm:f>NoModificar!$A$1:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>B2:B3 B5:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{95B98AD1-102E-4FDA-BE49-B30F33CA6C35}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1134F275-2622-4D4E-A45D-A5A39AF34C7E}">
           <x14:formula1>
             <xm:f>NoModificar!$C$1:$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>N2:N1048576</xm:sqref>
+          <xm:sqref>N2:N3 N5:N1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0018B0BB-D45A-4921-A724-A307D616D8E8}">
+        <x14:dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2353FA25-FE12-4F6C-BDCD-CCEF3BE3AC47}">
           <x14:formula1>
             <xm:f>NoModificar!D1</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
+          <xm:sqref>M2:M3 M6:M1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6752BDFC-61FA-41ED-9D4A-1854B80104FB}">
+        <x14:dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D02F09DA-9F19-4130-BB05-4BB2B628A3D6}">
+          <x14:formula1>
+            <xm:f>NoModificar!D3</xm:f>
+          </x14:formula1>
+          <xm:sqref>M5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5936CA36-E710-4595-957F-9EFBD03F890E}">
           <x14:formula1>
             <xm:f>NoModificar!$B$1:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F2:F3 F5:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -847,7 +895,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44339</v>
+        <v>44341</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Planilla ingresa despachos con prefijo TEST
</commit_message>
<xml_diff>
--- a/PlanillaDespachos.xlsx
+++ b/PlanillaDespachos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Home\Documents\beetrackManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45380059-5081-4C8E-B971-F1CAD3DC4A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA12A306-564A-4EAE-8773-07A887977B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3D032C6-7964-4F1D-846B-5E1174383D11}"/>
+    <workbookView xWindow="2400" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{B3D032C6-7964-4F1D-846B-5E1174383D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Despachos" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="N2" s="7">
         <f ca="1">TODAY()+1</f>
-        <v>44348</v>
+        <v>44350</v>
       </c>
       <c r="O2" t="s">
         <v>22</v>
@@ -777,7 +777,7 @@
       </c>
       <c r="N3" s="7">
         <f ca="1">TODAY()+2</f>
-        <v>44349</v>
+        <v>44351</v>
       </c>
       <c r="O3" t="s">
         <v>21</v>
@@ -908,7 +908,7 @@
       </c>
       <c r="D1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44347</v>
+        <v>44349</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>